<commit_message>
some changes in second years pic
</commit_message>
<xml_diff>
--- a/img/team/team second year.xlsx
+++ b/img/team/team second year.xlsx
@@ -1,17 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="600" yWindow="495" windowWidth="14055" windowHeight="4305"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Form responses 1" sheetId="1" r:id="rId3"/>
+    <sheet name="Form responses 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="122">
   <si>
     <t>Email address</t>
   </si>
@@ -148,9 +151,6 @@
     <t>Ankita Tirkey</t>
   </si>
   <si>
-    <t>https://m.facebook.com/photo.php?fbid=2050468265274269&amp;id=100009333471363&amp;set=a.1412953159025786&amp;source=11</t>
-  </si>
-  <si>
     <t>ashasmitanayakrkl@gmail.com</t>
   </si>
   <si>
@@ -368,25 +368,48 @@
   </si>
   <si>
     <t>https://www.linkedin.com/in/ramendranath-polai-b65130173/</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/soumik.patnaik.9</t>
+  </si>
+  <si>
+    <t>Abhishek Agrawal</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/abhishek-agrawal-41a171173/</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/anita.ktirkey</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -394,61 +417,343 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="3.29"/>
-    <col customWidth="1" min="2" max="3" width="21.57"/>
-    <col customWidth="1" min="4" max="4" width="73.14"/>
-    <col customWidth="1" min="5" max="5" width="35.0"/>
-    <col customWidth="1" min="6" max="12" width="21.57"/>
+    <col min="1" max="1" width="3.28515625" customWidth="1"/>
+    <col min="2" max="3" width="21.5703125" customWidth="1"/>
+    <col min="4" max="4" width="73.140625" customWidth="1"/>
+    <col min="5" max="5" width="35" customWidth="1"/>
+    <col min="6" max="12" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -465,7 +770,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -483,7 +788,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="2" t="s">
         <v>10</v>
@@ -501,7 +806,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="2" t="s">
         <v>15</v>
@@ -513,7 +818,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1">
       <c r="A5" s="1"/>
       <c r="B5" s="2" t="s">
         <v>18</v>
@@ -528,7 +833,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1">
       <c r="A6" s="1"/>
       <c r="B6" s="2" t="s">
         <v>22</v>
@@ -546,7 +851,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="2" t="s">
         <v>26</v>
@@ -561,7 +866,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="2" t="s">
         <v>29</v>
@@ -576,7 +881,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="2" t="s">
         <v>32</v>
@@ -594,7 +899,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="2" t="s">
         <v>36</v>
@@ -609,7 +914,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1">
       <c r="A11" s="1"/>
       <c r="B11" s="2" t="s">
         <v>39</v>
@@ -627,7 +932,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1">
       <c r="A12" s="1"/>
       <c r="B12" s="2" t="s">
         <v>43</v>
@@ -636,428 +941,442 @@
         <v>44</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>45</v>
+        <v>121</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1">
       <c r="A13" s="1"/>
       <c r="B13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:6" ht="15.75" customHeight="1">
       <c r="A14" s="1"/>
       <c r="B14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="F14" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:6" ht="15.75" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="F15" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:6" ht="15.75" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:6" ht="15.75" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="F17" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:6" ht="15.75" customHeight="1">
       <c r="A18" s="1"/>
       <c r="B18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="F18" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:6" ht="15.75" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="F19" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:6" ht="15.75" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="E20" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:6" ht="15.75" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="E21" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>70</v>
-      </c>
       <c r="F21" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:6" ht="15.75" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>73</v>
-      </c>
       <c r="F22" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:6" ht="15.75" customHeight="1">
       <c r="A23" s="1"/>
       <c r="B23" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:6" ht="15.75" customHeight="1">
       <c r="A24" s="1"/>
       <c r="B24" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:6" ht="15.75" customHeight="1">
       <c r="A25" s="1"/>
       <c r="B25" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="F25" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:6" ht="15.75" customHeight="1">
       <c r="A26" s="1"/>
       <c r="B26" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>82</v>
+      <c r="D26" t="s">
+        <v>118</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:6" ht="15.75" customHeight="1">
       <c r="A27" s="1"/>
       <c r="B27" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="D27" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="E27" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>86</v>
-      </c>
       <c r="F27" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:6" ht="15.75" customHeight="1">
       <c r="A28" s="1"/>
       <c r="B28" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="E28" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:6" ht="15.75" customHeight="1">
       <c r="A29" s="1"/>
       <c r="B29" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="D29" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>92</v>
-      </c>
       <c r="F29" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:6" ht="15.75" customHeight="1">
       <c r="A30" s="1"/>
       <c r="B30" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="F30" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:6" ht="15.75" customHeight="1">
       <c r="A31" s="1"/>
       <c r="B31" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="D31" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>97</v>
-      </c>
       <c r="F31" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:6" ht="15.75" customHeight="1">
       <c r="A32" s="1"/>
       <c r="B32" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="D32" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="F32" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:6" ht="15.75" customHeight="1">
       <c r="A33" s="1"/>
       <c r="B33" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="E33" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:6" ht="15.75" customHeight="1">
       <c r="A34" s="1"/>
       <c r="B34" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="D34" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="E34" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E34" s="3" t="s">
-        <v>107</v>
-      </c>
       <c r="F34" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:6" ht="15.75" customHeight="1">
       <c r="A35" s="1"/>
       <c r="B35" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="D35" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="E35" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>111</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:6" ht="15.75" customHeight="1">
       <c r="A36" s="1"/>
       <c r="B36" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="D36" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>114</v>
-      </c>
       <c r="F36" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:6" ht="15.75" customHeight="1">
       <c r="A37" s="1"/>
       <c r="B37" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="D37" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="E37" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="E37" s="3" t="s">
-        <v>118</v>
-      </c>
       <c r="F37" s="2" t="s">
         <v>17</v>
       </c>
+    </row>
+    <row r="38" spans="1:6" ht="15.75" customHeight="1">
+      <c r="C38" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E38" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="15.75" customHeight="1">
+      <c r="C39" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="D2"/>
-    <hyperlink r:id="rId2" ref="E2"/>
-    <hyperlink r:id="rId3" ref="D3"/>
-    <hyperlink r:id="rId4" ref="E3"/>
-    <hyperlink r:id="rId5" ref="D5"/>
-    <hyperlink r:id="rId6" ref="D6"/>
-    <hyperlink r:id="rId7" ref="E6"/>
-    <hyperlink r:id="rId8" ref="D7"/>
-    <hyperlink r:id="rId9" ref="D8"/>
-    <hyperlink r:id="rId10" ref="D9"/>
-    <hyperlink r:id="rId11" ref="E9"/>
-    <hyperlink r:id="rId12" ref="D10"/>
-    <hyperlink r:id="rId13" ref="D11"/>
-    <hyperlink r:id="rId14" ref="E11"/>
-    <hyperlink r:id="rId15" ref="D12"/>
-    <hyperlink r:id="rId16" ref="D14"/>
-    <hyperlink r:id="rId17" ref="D15"/>
-    <hyperlink r:id="rId18" ref="D17"/>
-    <hyperlink r:id="rId19" ref="D18"/>
-    <hyperlink r:id="rId20" ref="E20"/>
-    <hyperlink r:id="rId21" ref="D21"/>
-    <hyperlink r:id="rId22" ref="E21"/>
-    <hyperlink r:id="rId23" ref="D22"/>
-    <hyperlink r:id="rId24" ref="D23"/>
-    <hyperlink r:id="rId25" ref="D27"/>
-    <hyperlink r:id="rId26" ref="E27"/>
-    <hyperlink r:id="rId27" ref="E28"/>
-    <hyperlink r:id="rId28" ref="D29"/>
-    <hyperlink r:id="rId29" ref="D31"/>
-    <hyperlink r:id="rId30" ref="D32"/>
-    <hyperlink r:id="rId31" ref="E33"/>
-    <hyperlink r:id="rId32" ref="D34"/>
-    <hyperlink r:id="rId33" ref="E34"/>
-    <hyperlink r:id="rId34" ref="D35"/>
-    <hyperlink r:id="rId35" ref="E35"/>
-    <hyperlink r:id="rId36" ref="D36"/>
-    <hyperlink r:id="rId37" ref="D37"/>
-    <hyperlink r:id="rId38" ref="E37"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="D3" r:id="rId3"/>
+    <hyperlink ref="E3" r:id="rId4"/>
+    <hyperlink ref="D5" r:id="rId5"/>
+    <hyperlink ref="D6" r:id="rId6"/>
+    <hyperlink ref="E6" r:id="rId7"/>
+    <hyperlink ref="D7" r:id="rId8"/>
+    <hyperlink ref="D8" r:id="rId9"/>
+    <hyperlink ref="D9" r:id="rId10"/>
+    <hyperlink ref="E9" r:id="rId11"/>
+    <hyperlink ref="D10" r:id="rId12"/>
+    <hyperlink ref="D11" r:id="rId13"/>
+    <hyperlink ref="E11" r:id="rId14"/>
+    <hyperlink ref="D14" r:id="rId15"/>
+    <hyperlink ref="D15" r:id="rId16"/>
+    <hyperlink ref="D17" r:id="rId17"/>
+    <hyperlink ref="D18" r:id="rId18"/>
+    <hyperlink ref="E20" r:id="rId19"/>
+    <hyperlink ref="D21" r:id="rId20"/>
+    <hyperlink ref="E21" r:id="rId21"/>
+    <hyperlink ref="D22" r:id="rId22"/>
+    <hyperlink ref="D23" r:id="rId23"/>
+    <hyperlink ref="D27" r:id="rId24"/>
+    <hyperlink ref="E27" r:id="rId25"/>
+    <hyperlink ref="E28" r:id="rId26"/>
+    <hyperlink ref="D29" r:id="rId27"/>
+    <hyperlink ref="D31" r:id="rId28"/>
+    <hyperlink ref="D32" r:id="rId29"/>
+    <hyperlink ref="E33" r:id="rId30"/>
+    <hyperlink ref="D34" r:id="rId31"/>
+    <hyperlink ref="E34" r:id="rId32"/>
+    <hyperlink ref="D35" r:id="rId33"/>
+    <hyperlink ref="E35" r:id="rId34"/>
+    <hyperlink ref="D36" r:id="rId35"/>
+    <hyperlink ref="D37" r:id="rId36"/>
+    <hyperlink ref="E37" r:id="rId37"/>
   </hyperlinks>
-  <drawing r:id="rId39"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId38"/>
 </worksheet>
 </file>
</xml_diff>